<commit_message>
[FIX] update data formatting for consistency
</commit_message>
<xml_diff>
--- a/financial_data/iQPS.xlsx
+++ b/financial_data/iQPS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shinten/Desktop/space_econometrics/financial_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF18578-0380-8844-A041-4A42B6C799D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E003C1E-6178-4B82-B2BB-3FA980658DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4900" yWindow="1340" windowWidth="20040" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10005" yWindow="4605" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="income" sheetId="2" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>Fixed Assets</t>
   </si>
   <si>
-    <t>Current Liabilities</t>
-  </si>
-  <si>
     <t>Fixed Liabilities</t>
   </si>
   <si>
@@ -53,10 +50,6 @@
     <t>Capital Surplus</t>
   </si>
   <si>
-    <t>Equity</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Translation Adjustments</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -65,14 +58,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Total Liabilities and Equity</t>
-  </si>
-  <si>
     <t>Retained Earnings</t>
-  </si>
-  <si>
-    <t>Current Assets</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Total Assets</t>
@@ -81,13 +67,25 @@
   <si>
     <t>Quarter</t>
   </si>
+  <si>
+    <t>Total Current Assets</t>
+  </si>
+  <si>
+    <t>Total Current Liabilities</t>
+  </si>
+  <si>
+    <t>Total Equity</t>
+  </si>
+  <si>
+    <t>Liabilities and Equity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;¥&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;¥&quot;#,##0"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -189,14 +187,14 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -504,73 +502,73 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N18"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" customWidth="1"/>
-    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="20">
+    <row r="1" spans="1:18" ht="19.5">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18" ht="20">
+    <row r="2" spans="1:18" ht="19.5">
       <c r="A2" s="4">
         <v>43556</v>
       </c>
@@ -620,7 +618,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="18">
+    <row r="3" spans="1:18" ht="18.75">
       <c r="A3" s="5">
         <v>43647</v>
       </c>
@@ -681,7 +679,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="8"/>
     </row>
-    <row r="4" spans="1:18" ht="18">
+    <row r="4" spans="1:18" ht="18.75">
       <c r="A4" s="5">
         <v>43739</v>
       </c>
@@ -742,7 +740,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="8"/>
     </row>
-    <row r="5" spans="1:18" ht="18">
+    <row r="5" spans="1:18" ht="18.75">
       <c r="A5" s="5">
         <v>43831</v>
       </c>
@@ -803,7 +801,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="8"/>
     </row>
-    <row r="6" spans="1:18" ht="20">
+    <row r="6" spans="1:18" ht="19.5">
       <c r="A6" s="4">
         <v>43922</v>
       </c>
@@ -851,7 +849,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" ht="18">
+    <row r="7" spans="1:18" ht="18.75">
       <c r="A7" s="5">
         <v>44013</v>
       </c>
@@ -904,7 +902,7 @@
         <v>824938.54520547949</v>
       </c>
       <c r="N7" s="12">
-        <f t="shared" ref="N7:R7" si="11">(N6-N8)/($A8-$A6)*($A8-$A7)+N8</f>
+        <f t="shared" ref="N7" si="11">(N6-N8)/($A8-$A6)*($A8-$A7)+N8</f>
         <v>931026.30410958908</v>
       </c>
       <c r="O7" s="6"/>
@@ -912,7 +910,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="9"/>
     </row>
-    <row r="8" spans="1:18" ht="18">
+    <row r="8" spans="1:18" ht="18.75">
       <c r="A8" s="5">
         <v>44105</v>
       </c>
@@ -925,7 +923,7 @@
         <v>8606.1780821917819</v>
       </c>
       <c r="D8" s="12">
-        <f t="shared" ref="D8:O8" si="12">(D6-D10)/($A10-$A6)*($A10-$A8)+D10</f>
+        <f t="shared" ref="D8:N8" si="12">(D6-D10)/($A10-$A6)*($A10-$A8)+D10</f>
         <v>990990.39178082196</v>
       </c>
       <c r="E8" s="12">
@@ -973,7 +971,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="9"/>
     </row>
-    <row r="9" spans="1:18" ht="18">
+    <row r="9" spans="1:18" ht="18.75">
       <c r="A9" s="5">
         <v>44197</v>
       </c>
@@ -1026,7 +1024,7 @@
         <v>791969.27397260279</v>
       </c>
       <c r="N9" s="12">
-        <f t="shared" ref="N9:R9" si="20">(N8-N10)/($A10-$A8)*($A10-$A9)+N10</f>
+        <f t="shared" ref="N9" si="20">(N8-N10)/($A10-$A8)*($A10-$A9)+N10</f>
         <v>1050954.4794520547</v>
       </c>
       <c r="O9" s="6"/>
@@ -1034,7 +1032,7 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="1:18" ht="20">
+    <row r="10" spans="1:18" ht="19.5">
       <c r="A10" s="4">
         <v>44287</v>
       </c>
@@ -1082,7 +1080,7 @@
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" ht="18">
+    <row r="11" spans="1:18" ht="18.75">
       <c r="A11" s="5">
         <v>44378</v>
       </c>
@@ -1135,7 +1133,7 @@
         <v>1899602.9972602739</v>
       </c>
       <c r="N11" s="12">
-        <f t="shared" ref="N11:R11" si="28">(N10-N12)/($A12-$A10)*($A12-$A11)+N12</f>
+        <f t="shared" ref="N11" si="28">(N10-N12)/($A12-$A10)*($A12-$A11)+N12</f>
         <v>2245336.6356164385</v>
       </c>
       <c r="O11" s="6"/>
@@ -1143,7 +1141,7 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="9"/>
     </row>
-    <row r="12" spans="1:18" ht="18">
+    <row r="12" spans="1:18" ht="18.75">
       <c r="A12" s="5">
         <v>44470</v>
       </c>
@@ -1156,7 +1154,7 @@
         <v>956126.75068493153</v>
       </c>
       <c r="D12" s="12">
-        <f t="shared" ref="D12:R12" si="29">(D10-D14)/($A14-$A10)*($A14-$A12)+D14</f>
+        <f t="shared" ref="D12:N12" si="29">(D10-D14)/($A14-$A10)*($A14-$A12)+D14</f>
         <v>3393538.7287671231</v>
       </c>
       <c r="E12" s="12">
@@ -1204,7 +1202,7 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="9"/>
     </row>
-    <row r="13" spans="1:18" ht="18">
+    <row r="13" spans="1:18" ht="18.75">
       <c r="A13" s="5">
         <v>44562</v>
       </c>
@@ -1257,7 +1255,7 @@
         <v>4171821.01369863</v>
       </c>
       <c r="N13" s="12">
-        <f t="shared" ref="N13:R13" si="37">(N12-N14)/($A14-$A12)*($A14-$A13)+N14</f>
+        <f t="shared" ref="N13" si="37">(N12-N14)/($A14-$A12)*($A14-$A13)+N14</f>
         <v>4541740.8219178077</v>
       </c>
       <c r="O13" s="6"/>
@@ -1265,7 +1263,7 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="9"/>
     </row>
-    <row r="14" spans="1:18" ht="20">
+    <row r="14" spans="1:18" ht="19.5">
       <c r="A14" s="4">
         <v>44652</v>
       </c>
@@ -1313,7 +1311,7 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" ht="18">
+    <row r="15" spans="1:18" ht="18.75">
       <c r="A15" s="5">
         <v>44743</v>
       </c>
@@ -1354,7 +1352,7 @@
         <v>5894264.6986301374</v>
       </c>
       <c r="K15" s="12">
-        <f t="shared" ref="K15:R15" si="44">(K14-K16)/($A16-$A14)*($A16-$A15)+K16</f>
+        <f t="shared" ref="K15:M15" si="44">(K14-K16)/($A16-$A14)*($A16-$A15)+K16</f>
         <v>-662773.76438356168</v>
       </c>
       <c r="L15" s="12">
@@ -1374,7 +1372,7 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="9"/>
     </row>
-    <row r="16" spans="1:18" ht="18">
+    <row r="16" spans="1:18" ht="18.75">
       <c r="A16" s="5">
         <v>44835</v>
       </c>
@@ -1435,7 +1433,7 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="9"/>
     </row>
-    <row r="17" spans="1:18" ht="18">
+    <row r="17" spans="1:18" ht="18.75">
       <c r="A17" s="5">
         <v>44927</v>
       </c>
@@ -1476,7 +1474,7 @@
         <v>6353014.506849315</v>
       </c>
       <c r="K17" s="12">
-        <f t="shared" ref="K17:R17" si="54">(K16-K18)/($A18-$A16)*($A18-$A17)+K18</f>
+        <f t="shared" ref="K17:M17" si="54">(K16-K18)/($A18-$A16)*($A18-$A17)+K18</f>
         <v>-1219915.1780821919</v>
       </c>
       <c r="L17" s="12">
@@ -1496,7 +1494,7 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="9"/>
     </row>
-    <row r="18" spans="1:18" ht="20">
+    <row r="18" spans="1:18" ht="19.5">
       <c r="A18" s="4">
         <v>45017</v>
       </c>

</xml_diff>

<commit_message>
[DATA] remove rows in iQPS data which do not have complete data
</commit_message>
<xml_diff>
--- a/financial_data/iQPS.xlsx
+++ b/financial_data/iQPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5DA2EB-0F79-471A-9652-205E8F37EAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D91BD2-10A4-45CB-8D91-7CA0B40C4DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -237,15 +237,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -550,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECC31B8-9403-4F66-B332-2C0CDF711F8B}">
-  <dimension ref="A1:AG27"/>
+  <dimension ref="A1:AG23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+      <selection activeCell="A19" sqref="A19:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2408,259 +2399,17 @@
         <v>-1105199000</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="15">
-      <c r="A19" s="10">
-        <v>45169</v>
-      </c>
-      <c r="B19" s="11">
-        <v>3</v>
-      </c>
-      <c r="C19" s="11">
-        <v>2</v>
-      </c>
-      <c r="D19" s="9">
-        <v>3031637846.9945354</v>
-      </c>
-      <c r="E19" s="9">
-        <v>2974348857.9234972</v>
-      </c>
-      <c r="F19" s="9">
-        <v>6039474699.4535522</v>
-      </c>
-      <c r="G19" s="9">
-        <v>470637426.22950816</v>
-      </c>
-      <c r="H19" s="9">
-        <v>456173508.19672132</v>
-      </c>
-      <c r="I19" s="9">
-        <v>926811934.42622948</v>
-      </c>
-      <c r="J19" s="9">
-        <v>5102310251.3661203</v>
-      </c>
-      <c r="K19" s="9">
-        <v>100000000</v>
-      </c>
-      <c r="L19" s="9">
-        <v>5827109819.6721306</v>
-      </c>
-      <c r="M19" s="9">
-        <v>-824799071.0382514</v>
-      </c>
-      <c r="N19" s="9">
-        <v>2970994464.4808745</v>
-      </c>
-      <c r="O19" s="9">
-        <v>5112662765.0273228</v>
-      </c>
-      <c r="P19" s="9">
-        <v>6039474699.4535522</v>
-      </c>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="2"/>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="2"/>
-      <c r="AD19" s="2"/>
-      <c r="AE19" s="2"/>
-      <c r="AF19" s="2"/>
-      <c r="AG19" s="2"/>
+    <row r="20" spans="1:33">
+      <c r="D20" s="4"/>
     </row>
-    <row r="20" spans="1:33" ht="15">
-      <c r="A20" s="10">
-        <v>45260</v>
-      </c>
-      <c r="B20" s="11">
-        <v>3</v>
-      </c>
-      <c r="C20" s="11">
-        <v>2</v>
-      </c>
-      <c r="D20" s="9">
-        <v>2207696000</v>
-      </c>
-      <c r="E20" s="9">
-        <v>3969590000</v>
-      </c>
-      <c r="F20" s="9">
-        <v>6243897000</v>
-      </c>
-      <c r="G20" s="9">
-        <v>614404000</v>
-      </c>
-      <c r="H20" s="9">
-        <v>603049000</v>
-      </c>
-      <c r="I20" s="9">
-        <v>1217454000</v>
-      </c>
-      <c r="J20" s="9">
-        <v>5020547000</v>
-      </c>
-      <c r="K20" s="9">
-        <v>100000000</v>
-      </c>
-      <c r="L20" s="9">
-        <v>5084972000</v>
-      </c>
-      <c r="M20" s="9">
-        <v>-164425000</v>
-      </c>
-      <c r="N20" s="9">
-        <v>5895000000</v>
-      </c>
-      <c r="O20" s="9">
-        <v>5026443000</v>
-      </c>
-      <c r="P20" s="9">
-        <v>6243897000</v>
-      </c>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="2"/>
-      <c r="AD20" s="2"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="2"/>
-      <c r="AG20" s="2"/>
+    <row r="21" spans="1:33">
+      <c r="D21" s="4"/>
     </row>
-    <row r="21" spans="1:33" ht="15">
-      <c r="A21" s="10">
-        <v>45351</v>
-      </c>
-      <c r="B21" s="11">
-        <v>4</v>
-      </c>
-      <c r="C21" s="11">
-        <v>3</v>
-      </c>
-      <c r="D21" s="9">
-        <v>5351940000</v>
-      </c>
-      <c r="E21" s="9">
-        <v>4828566000</v>
-      </c>
-      <c r="F21" s="9">
-        <v>10180507000</v>
-      </c>
-      <c r="G21" s="9">
-        <v>688123000</v>
-      </c>
-      <c r="H21" s="9">
-        <v>610908000</v>
-      </c>
-      <c r="I21" s="9">
-        <v>1299032000</v>
-      </c>
-      <c r="J21" s="9">
-        <v>8856571000</v>
-      </c>
-      <c r="K21" s="9">
-        <v>1939980000</v>
-      </c>
-      <c r="L21" s="9">
-        <v>6924953000</v>
-      </c>
-      <c r="M21" s="9">
-        <v>-8361000</v>
-      </c>
-      <c r="N21" s="9">
-        <v>24903000</v>
-      </c>
-      <c r="O21" s="9">
-        <v>8881475000</v>
-      </c>
-      <c r="P21" s="9">
-        <v>10180507000</v>
-      </c>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="2"/>
-      <c r="AD21" s="2"/>
-      <c r="AE21" s="2"/>
-      <c r="AF21" s="2"/>
-      <c r="AG21" s="2"/>
+    <row r="22" spans="1:33">
+      <c r="D22" s="4"/>
     </row>
-    <row r="22" spans="1:33" ht="15">
-      <c r="A22" s="10">
-        <v>45443</v>
-      </c>
-      <c r="B22" s="11">
-        <v>5</v>
-      </c>
-      <c r="C22" s="11">
-        <v>3</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="2"/>
-      <c r="Z22" s="2"/>
-      <c r="AA22" s="2"/>
-      <c r="AB22" s="2"/>
-      <c r="AC22" s="2"/>
-      <c r="AD22" s="2"/>
-      <c r="AE22" s="2"/>
-      <c r="AF22" s="2"/>
-      <c r="AG22" s="2"/>
-    </row>
-    <row r="24" spans="1:33">
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:33">
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:33">
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:33">
-      <c r="D27" s="4"/>
+    <row r="23" spans="1:33">
+      <c r="D23" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
[DATA] iQPS data consistent formatting / consolidation
</commit_message>
<xml_diff>
--- a/financial_data/iQPS.xlsx
+++ b/financial_data/iQPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D91BD2-10A4-45CB-8D91-7CA0B40C4DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C14CDA2-98D4-4743-BD49-2AD0A42D4FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,10 +149,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="&quot;¥&quot;#,##0"/>
-    <numFmt numFmtId="165" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
     <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="170" formatCode="_-[$¥-411]* #,##0_-;\-[$¥-411]* #,##0_-;_-[$¥-411]* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -210,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -227,18 +228,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,41 +546,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECC31B8-9403-4F66-B332-2C0CDF711F8B}">
   <dimension ref="A1:AG23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD22"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="18.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="34" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
@@ -683,13 +684,13 @@
       </c>
     </row>
     <row r="2" spans="1:33" ht="15">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <v>43616</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>0</v>
       </c>
       <c r="D2" s="8">
@@ -784,13 +785,13 @@
       </c>
     </row>
     <row r="3" spans="1:33" ht="15">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <v>43708</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>0</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>0</v>
       </c>
       <c r="D3" s="8">
@@ -885,13 +886,13 @@
       </c>
     </row>
     <row r="4" spans="1:33" ht="15">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <v>43799</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>0</v>
       </c>
       <c r="D4" s="8">
@@ -986,13 +987,13 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="15">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <v>43888</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>0</v>
       </c>
       <c r="D5" s="8">
@@ -1087,13 +1088,13 @@
       </c>
     </row>
     <row r="6" spans="1:33" ht="15">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <v>43982</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>1</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>0</v>
       </c>
       <c r="D6" s="8">
@@ -1188,13 +1189,13 @@
       </c>
     </row>
     <row r="7" spans="1:33" ht="15">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <v>44074</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>1</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0</v>
       </c>
       <c r="D7" s="8">
@@ -1289,13 +1290,13 @@
       </c>
     </row>
     <row r="8" spans="1:33" ht="15">
-      <c r="A8" s="6">
+      <c r="A8" s="7">
         <v>44165</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>0</v>
       </c>
       <c r="D8" s="8">
@@ -1390,13 +1391,13 @@
       </c>
     </row>
     <row r="9" spans="1:33" ht="15">
-      <c r="A9" s="6">
+      <c r="A9" s="7">
         <v>44254</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>0</v>
       </c>
       <c r="D9" s="8">
@@ -1491,13 +1492,13 @@
       </c>
     </row>
     <row r="10" spans="1:33" ht="15">
-      <c r="A10" s="6">
+      <c r="A10" s="7">
         <v>44347</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>2</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>1</v>
       </c>
       <c r="D10" s="8">
@@ -1542,7 +1543,7 @@
       <c r="Q10" s="9">
         <v>4300000</v>
       </c>
-      <c r="R10" s="9">
+      <c r="R10" s="8">
         <v>-4220000</v>
       </c>
       <c r="S10" s="9">
@@ -1592,13 +1593,13 @@
       </c>
     </row>
     <row r="11" spans="1:33" ht="15">
-      <c r="A11" s="6">
+      <c r="A11" s="7">
         <v>44439</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>2</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>1</v>
       </c>
       <c r="D11" s="8">
@@ -1693,13 +1694,13 @@
       </c>
     </row>
     <row r="12" spans="1:33" ht="15">
-      <c r="A12" s="6">
+      <c r="A12" s="7">
         <v>44530</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>1</v>
       </c>
       <c r="D12" s="8">
@@ -1794,13 +1795,13 @@
       </c>
     </row>
     <row r="13" spans="1:33" ht="15">
-      <c r="A13" s="6">
+      <c r="A13" s="7">
         <v>44619</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>2</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>1</v>
       </c>
       <c r="D13" s="8">
@@ -1895,13 +1896,13 @@
       </c>
     </row>
     <row r="14" spans="1:33" ht="15">
-      <c r="A14" s="6">
+      <c r="A14" s="7">
         <v>44712</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>2</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>1</v>
       </c>
       <c r="D14" s="8">
@@ -1996,13 +1997,13 @@
       </c>
     </row>
     <row r="15" spans="1:33" ht="15">
-      <c r="A15" s="6">
+      <c r="A15" s="7">
         <v>44804</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>2</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>1</v>
       </c>
       <c r="D15" s="8">
@@ -2097,13 +2098,13 @@
       </c>
     </row>
     <row r="16" spans="1:33" ht="15">
-      <c r="A16" s="6">
+      <c r="A16" s="7">
         <v>44895</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>2</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>1</v>
       </c>
       <c r="D16" s="8">
@@ -2198,13 +2199,13 @@
       </c>
     </row>
     <row r="17" spans="1:33" ht="15">
-      <c r="A17" s="6">
+      <c r="A17" s="7">
         <v>44984</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>1</v>
       </c>
       <c r="D17" s="8">
@@ -2299,13 +2300,13 @@
       </c>
     </row>
     <row r="18" spans="1:33" ht="15">
-      <c r="A18" s="6">
+      <c r="A18" s="7">
         <v>45077</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>2</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>1</v>
       </c>
       <c r="D18" s="8">
@@ -2326,7 +2327,7 @@
       <c r="I18" s="8">
         <v>632976000</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="8">
         <v>5184972000</v>
       </c>
       <c r="K18" s="8">
@@ -2347,66 +2348,299 @@
       <c r="P18" s="8">
         <v>5832806000</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="Q18" s="8">
         <v>372072000</v>
       </c>
-      <c r="R18" s="9">
+      <c r="R18" s="8">
         <v>-215197000</v>
       </c>
-      <c r="S18" s="9">
+      <c r="S18" s="8">
         <v>156875000</v>
       </c>
-      <c r="T18" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U18" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="V18" s="9">
+      <c r="T18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="U18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="V18" s="8">
         <v>471595000</v>
       </c>
-      <c r="W18" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="X18" s="9">
+      <c r="W18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="X18" s="8">
         <v>-314720000</v>
       </c>
-      <c r="Y18" s="9">
+      <c r="Y18" s="8">
         <v>-4796000</v>
       </c>
-      <c r="Z18" s="9">
+      <c r="Z18" s="8">
         <v>37000</v>
       </c>
-      <c r="AA18" s="9">
+      <c r="AA18" s="8">
         <v>-1499000</v>
       </c>
-      <c r="AB18" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC18" s="9">
+      <c r="AB18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC18" s="8">
         <v>242000</v>
       </c>
-      <c r="AD18" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE18" s="9">
+      <c r="AD18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE18" s="8">
         <v>-1103861000</v>
       </c>
-      <c r="AF18" s="9">
+      <c r="AF18" s="8">
         <v>1337000</v>
       </c>
-      <c r="AG18" s="9">
+      <c r="AG18" s="8">
         <v>-1105199000</v>
       </c>
     </row>
-    <row r="20" spans="1:33">
-      <c r="D20" s="4"/>
+    <row r="19" spans="1:33" customFormat="1" ht="15">
+      <c r="A19" s="7">
+        <v>45169</v>
+      </c>
+      <c r="B19" s="6">
+        <v>3</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="8">
+        <v>3031637846.9945354</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2974348857.9234972</v>
+      </c>
+      <c r="F19" s="8">
+        <v>6039474699.4535522</v>
+      </c>
+      <c r="G19" s="8">
+        <v>470637426.22950816</v>
+      </c>
+      <c r="H19" s="8">
+        <v>456173508.19672132</v>
+      </c>
+      <c r="I19" s="8">
+        <v>926811934.42622948</v>
+      </c>
+      <c r="J19" s="8">
+        <v>5102310251.3661203</v>
+      </c>
+      <c r="K19" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="L19" s="8">
+        <v>5827109819.6721306</v>
+      </c>
+      <c r="M19" s="8">
+        <v>-824799071.0382514</v>
+      </c>
+      <c r="N19" s="8">
+        <v>2970994464.4808745</v>
+      </c>
+      <c r="O19" s="8">
+        <v>5112662765.0273228</v>
+      </c>
+      <c r="P19" s="8">
+        <v>6039474699.4535522</v>
+      </c>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
+      <c r="AC19" s="8"/>
+      <c r="AD19" s="8"/>
+      <c r="AE19" s="8"/>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
     </row>
-    <row r="21" spans="1:33">
-      <c r="D21" s="4"/>
+    <row r="20" spans="1:33" customFormat="1" ht="15">
+      <c r="A20" s="7">
+        <v>45260</v>
+      </c>
+      <c r="B20" s="6">
+        <v>3</v>
+      </c>
+      <c r="C20" s="6">
+        <v>2</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2207696000</v>
+      </c>
+      <c r="E20" s="8">
+        <v>3969590000</v>
+      </c>
+      <c r="F20" s="8">
+        <v>6243897000</v>
+      </c>
+      <c r="G20" s="8">
+        <v>614404000</v>
+      </c>
+      <c r="H20" s="8">
+        <v>603049000</v>
+      </c>
+      <c r="I20" s="8">
+        <v>1217454000</v>
+      </c>
+      <c r="J20" s="8">
+        <v>5020547000</v>
+      </c>
+      <c r="K20" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="L20" s="8">
+        <v>5084972000</v>
+      </c>
+      <c r="M20" s="8">
+        <v>-164425000</v>
+      </c>
+      <c r="N20" s="8">
+        <v>5895000000</v>
+      </c>
+      <c r="O20" s="8">
+        <v>5026443000</v>
+      </c>
+      <c r="P20" s="8">
+        <v>6243897000</v>
+      </c>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
     </row>
-    <row r="22" spans="1:33">
-      <c r="D22" s="4"/>
+    <row r="21" spans="1:33" customFormat="1" ht="15">
+      <c r="A21" s="7">
+        <v>45351</v>
+      </c>
+      <c r="B21" s="6">
+        <v>4</v>
+      </c>
+      <c r="C21" s="6">
+        <v>3</v>
+      </c>
+      <c r="D21" s="8">
+        <v>5351940000</v>
+      </c>
+      <c r="E21" s="8">
+        <v>4828566000</v>
+      </c>
+      <c r="F21" s="8">
+        <v>10180507000</v>
+      </c>
+      <c r="G21" s="8">
+        <v>688123000</v>
+      </c>
+      <c r="H21" s="8">
+        <v>610908000</v>
+      </c>
+      <c r="I21" s="8">
+        <v>1299032000</v>
+      </c>
+      <c r="J21" s="8">
+        <v>8856571000</v>
+      </c>
+      <c r="K21" s="8">
+        <v>1939980000</v>
+      </c>
+      <c r="L21" s="8">
+        <v>6924953000</v>
+      </c>
+      <c r="M21" s="8">
+        <v>-8361000</v>
+      </c>
+      <c r="N21" s="8">
+        <v>24903000</v>
+      </c>
+      <c r="O21" s="8">
+        <v>8881475000</v>
+      </c>
+      <c r="P21" s="8">
+        <v>10180507000</v>
+      </c>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="8"/>
+    </row>
+    <row r="22" spans="1:33" customFormat="1">
+      <c r="A22" s="7">
+        <v>45443</v>
+      </c>
+      <c r="B22" s="6">
+        <v>5</v>
+      </c>
+      <c r="C22" s="6">
+        <v>3</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="10"/>
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
     </row>
     <row r="23" spans="1:33">
       <c r="D23" s="4"/>

</xml_diff>

<commit_message>
[ADD] change '-' to '0' in iQPS empty columns
</commit_message>
<xml_diff>
--- a/financial_data/iQPS.xlsx
+++ b/financial_data/iQPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C14CDA2-98D4-4743-BD49-2AD0A42D4FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EC8051-5267-4CF4-BB99-B9470A98DC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Fixed Assets</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Net loss</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Debt extinguishment gain</t>
@@ -151,9 +148,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="&quot;¥&quot;#,##0"/>
-    <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="170" formatCode="_-[$¥-411]* #,##0_-;\-[$¥-411]* #,##0_-;_-[$¥-411]* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="_-[$¥-411]* #,##0_-;\-[$¥-411]* #,##0_-;_-[$¥-411]* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -228,20 +225,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,7 +543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECC31B8-9403-4F66-B332-2C0CDF711F8B}">
   <dimension ref="A1:AG23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
@@ -587,10 +586,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -608,10 +607,10 @@
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>2</v>
@@ -656,7 +655,7 @@
         <v>19</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>20</v>
@@ -671,7 +670,7 @@
         <v>23</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>24</v>
@@ -741,17 +740,17 @@
       <c r="S2" s="9">
         <v>0</v>
       </c>
-      <c r="T2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>27</v>
+      <c r="T2" s="9">
+        <v>0</v>
+      </c>
+      <c r="U2" s="9">
+        <v>0</v>
       </c>
       <c r="V2" s="9">
         <v>595194000</v>
       </c>
-      <c r="W2" s="9" t="s">
-        <v>27</v>
+      <c r="W2" s="9">
+        <v>0</v>
       </c>
       <c r="X2" s="9">
         <v>-595194000</v>
@@ -765,14 +764,14 @@
       <c r="AA2" s="9">
         <v>-1032000</v>
       </c>
-      <c r="AB2" s="9" t="s">
-        <v>27</v>
+      <c r="AB2" s="9">
+        <v>0</v>
       </c>
       <c r="AC2" s="9">
         <v>1129000</v>
       </c>
-      <c r="AD2" s="9" t="s">
-        <v>27</v>
+      <c r="AD2" s="9">
+        <v>0</v>
       </c>
       <c r="AE2" s="9">
         <v>-592244000</v>
@@ -842,17 +841,17 @@
       <c r="S3" s="9">
         <v>10054.644808743169</v>
       </c>
-      <c r="T3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>27</v>
+      <c r="T3" s="9">
+        <v>0</v>
+      </c>
+      <c r="U3" s="9">
+        <v>0</v>
       </c>
       <c r="V3" s="8">
         <v>671911724.04371583</v>
       </c>
-      <c r="W3" s="9" t="s">
-        <v>27</v>
+      <c r="W3" s="9">
+        <v>0</v>
       </c>
       <c r="X3" s="8">
         <v>-671911724.04371583</v>
@@ -866,14 +865,14 @@
       <c r="AA3" s="8">
         <v>-820163.93442622945</v>
       </c>
-      <c r="AB3" s="9" t="s">
-        <v>27</v>
+      <c r="AB3" s="9">
+        <v>0</v>
       </c>
       <c r="AC3" s="8">
         <v>854756.83060109289</v>
       </c>
-      <c r="AD3" s="9" t="s">
-        <v>27</v>
+      <c r="AD3" s="9">
+        <v>0</v>
       </c>
       <c r="AE3" s="8">
         <v>-669425426.22950828</v>
@@ -943,17 +942,17 @@
       <c r="S4" s="9">
         <v>20000</v>
       </c>
-      <c r="T4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U4" s="9" t="s">
-        <v>27</v>
+      <c r="T4" s="9">
+        <v>0</v>
+      </c>
+      <c r="U4" s="9">
+        <v>0</v>
       </c>
       <c r="V4" s="8">
         <v>749472500</v>
       </c>
-      <c r="W4" s="9" t="s">
-        <v>27</v>
+      <c r="W4" s="9">
+        <v>0</v>
       </c>
       <c r="X4" s="8">
         <v>-749472500</v>
@@ -967,14 +966,14 @@
       <c r="AA4" s="8">
         <v>-606000</v>
       </c>
-      <c r="AB4" s="9" t="s">
-        <v>27</v>
+      <c r="AB4" s="9">
+        <v>0</v>
       </c>
       <c r="AC4" s="8">
         <v>577500</v>
       </c>
-      <c r="AD4" s="9" t="s">
-        <v>27</v>
+      <c r="AD4" s="9">
+        <v>0</v>
       </c>
       <c r="AE4" s="8">
         <v>-747455000</v>
@@ -1044,17 +1043,17 @@
       <c r="S5" s="9">
         <v>29726.775956284153</v>
       </c>
-      <c r="T5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>27</v>
+      <c r="T5" s="9">
+        <v>0</v>
+      </c>
+      <c r="U5" s="9">
+        <v>0</v>
       </c>
       <c r="V5" s="8">
         <v>827033275.95628417</v>
       </c>
-      <c r="W5" s="9" t="s">
-        <v>27</v>
+      <c r="W5" s="9">
+        <v>0</v>
       </c>
       <c r="X5" s="8">
         <v>-827033275.95628417</v>
@@ -1068,14 +1067,14 @@
       <c r="AA5" s="8">
         <v>-391836.06557377049</v>
       </c>
-      <c r="AB5" s="9" t="s">
-        <v>27</v>
+      <c r="AB5" s="9">
+        <v>0</v>
       </c>
       <c r="AC5" s="8">
         <v>300243.16939890711</v>
       </c>
-      <c r="AD5" s="9" t="s">
-        <v>27</v>
+      <c r="AD5" s="9">
+        <v>0</v>
       </c>
       <c r="AE5" s="8">
         <v>-825484573.77049184</v>
@@ -1145,17 +1144,17 @@
       <c r="S6" s="9">
         <v>40000</v>
       </c>
-      <c r="T6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U6" s="9" t="s">
-        <v>27</v>
+      <c r="T6" s="9">
+        <v>0</v>
+      </c>
+      <c r="U6" s="9">
+        <v>0</v>
       </c>
       <c r="V6" s="9">
         <v>903751000</v>
       </c>
-      <c r="W6" s="9" t="s">
-        <v>27</v>
+      <c r="W6" s="9">
+        <v>0</v>
       </c>
       <c r="X6" s="9">
         <v>-903751000</v>
@@ -1169,14 +1168,14 @@
       <c r="AA6" s="9">
         <v>-180000</v>
       </c>
-      <c r="AB6" s="9" t="s">
-        <v>27</v>
+      <c r="AB6" s="9">
+        <v>0</v>
       </c>
       <c r="AC6" s="9">
         <v>26000</v>
       </c>
-      <c r="AD6" s="9" t="s">
-        <v>27</v>
+      <c r="AD6" s="9">
+        <v>0</v>
       </c>
       <c r="AE6" s="9">
         <v>-902666000</v>
@@ -1246,17 +1245,17 @@
       <c r="S7" s="9">
         <v>50082.191780821922</v>
       </c>
-      <c r="T7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U7" s="9" t="s">
-        <v>27</v>
+      <c r="T7" s="9">
+        <v>0</v>
+      </c>
+      <c r="U7" s="9">
+        <v>0</v>
       </c>
       <c r="V7" s="8">
         <v>834882200</v>
       </c>
-      <c r="W7" s="9" t="s">
-        <v>27</v>
+      <c r="W7" s="9">
+        <v>0</v>
       </c>
       <c r="X7" s="8">
         <v>-834862254.79452062</v>
@@ -1270,14 +1269,14 @@
       <c r="AA7" s="8">
         <v>-388926.02739726024</v>
       </c>
-      <c r="AB7" s="9" t="s">
-        <v>27</v>
+      <c r="AB7" s="9">
+        <v>0</v>
       </c>
       <c r="AC7" s="8">
         <v>547567.12328767113</v>
       </c>
-      <c r="AD7" s="9" t="s">
-        <v>27</v>
+      <c r="AD7" s="9">
+        <v>0</v>
       </c>
       <c r="AE7" s="8">
         <v>-834731383.56164384</v>
@@ -1347,17 +1346,17 @@
       <c r="S8" s="9">
         <v>60054.794520547948</v>
       </c>
-      <c r="T8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U8" s="9" t="s">
-        <v>27</v>
+      <c r="T8" s="9">
+        <v>0</v>
+      </c>
+      <c r="U8" s="9">
+        <v>0</v>
       </c>
       <c r="V8" s="8">
         <v>765256600</v>
       </c>
-      <c r="W8" s="9" t="s">
-        <v>27</v>
+      <c r="W8" s="9">
+        <v>0</v>
       </c>
       <c r="X8" s="8">
         <v>-765216490.41095889</v>
@@ -1371,14 +1370,14 @@
       <c r="AA8" s="8">
         <v>-600147.94520547951</v>
       </c>
-      <c r="AB8" s="9" t="s">
-        <v>27</v>
+      <c r="AB8" s="9">
+        <v>0</v>
       </c>
       <c r="AC8" s="8">
         <v>1074865.7534246575</v>
       </c>
-      <c r="AD8" s="9" t="s">
-        <v>27</v>
+      <c r="AD8" s="9">
+        <v>0</v>
       </c>
       <c r="AE8" s="8">
         <v>-766050232.87671232</v>
@@ -1448,17 +1447,17 @@
       <c r="S9" s="9">
         <v>69808.219178082189</v>
       </c>
-      <c r="T9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U9" s="9" t="s">
-        <v>27</v>
+      <c r="T9" s="9">
+        <v>0</v>
+      </c>
+      <c r="U9" s="9">
+        <v>0</v>
       </c>
       <c r="V9" s="8">
         <v>695631000</v>
       </c>
-      <c r="W9" s="9" t="s">
-        <v>27</v>
+      <c r="W9" s="9">
+        <v>0</v>
       </c>
       <c r="X9" s="8">
         <v>-695570726.02739716</v>
@@ -1472,14 +1471,14 @@
       <c r="AA9" s="8">
         <v>-811369.8630136986</v>
       </c>
-      <c r="AB9" s="9" t="s">
-        <v>27</v>
+      <c r="AB9" s="9">
+        <v>0</v>
       </c>
       <c r="AC9" s="8">
         <v>1602164.3835616438</v>
       </c>
-      <c r="AD9" s="9" t="s">
-        <v>27</v>
+      <c r="AD9" s="9">
+        <v>0</v>
       </c>
       <c r="AE9" s="8">
         <v>-697369082.19178081</v>
@@ -1549,17 +1548,17 @@
       <c r="S10" s="9">
         <v>80000</v>
       </c>
-      <c r="T10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U10" s="9" t="s">
-        <v>27</v>
+      <c r="T10" s="9">
+        <v>0</v>
+      </c>
+      <c r="U10" s="9">
+        <v>0</v>
       </c>
       <c r="V10" s="9">
         <v>627519000</v>
       </c>
-      <c r="W10" s="9" t="s">
-        <v>27</v>
+      <c r="W10" s="9">
+        <v>0</v>
       </c>
       <c r="X10" s="9">
         <v>-627439000</v>
@@ -1573,14 +1572,14 @@
       <c r="AA10" s="9">
         <v>-1018000</v>
       </c>
-      <c r="AB10" s="9" t="s">
-        <v>27</v>
+      <c r="AB10" s="9">
+        <v>0</v>
       </c>
       <c r="AC10" s="9">
         <v>2118000</v>
       </c>
-      <c r="AD10" s="9" t="s">
-        <v>27</v>
+      <c r="AD10" s="9">
+        <v>0</v>
       </c>
       <c r="AE10" s="9">
         <v>-630181000</v>
@@ -1650,17 +1649,17 @@
       <c r="S11" s="8">
         <v>2646698.6301369863</v>
       </c>
-      <c r="T11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U11" s="9" t="s">
-        <v>27</v>
+      <c r="T11" s="9">
+        <v>0</v>
+      </c>
+      <c r="U11" s="9">
+        <v>0</v>
       </c>
       <c r="V11" s="8">
         <v>569009989.04109585</v>
       </c>
-      <c r="W11" s="9" t="s">
-        <v>27</v>
+      <c r="W11" s="9">
+        <v>0</v>
       </c>
       <c r="X11" s="8">
         <v>-566363290.41095889</v>
@@ -1674,14 +1673,14 @@
       <c r="AA11" s="8">
         <v>-353076.71232876717</v>
       </c>
-      <c r="AB11" s="9" t="s">
-        <v>27</v>
+      <c r="AB11" s="9">
+        <v>0</v>
       </c>
       <c r="AC11" s="8">
         <v>1593690.4109589041</v>
       </c>
-      <c r="AD11" s="9" t="s">
-        <v>27</v>
+      <c r="AD11" s="9">
+        <v>0</v>
       </c>
       <c r="AE11" s="8">
         <v>-569277317.80821919</v>
@@ -1751,17 +1750,17 @@
       <c r="S12" s="8">
         <v>5241602.7397260265</v>
       </c>
-      <c r="T12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U12" s="9" t="s">
-        <v>27</v>
+      <c r="T12" s="9">
+        <v>0</v>
+      </c>
+      <c r="U12" s="9">
+        <v>0</v>
       </c>
       <c r="V12" s="8">
         <v>509858021.91780823</v>
       </c>
-      <c r="W12" s="9" t="s">
-        <v>27</v>
+      <c r="W12" s="9">
+        <v>0</v>
       </c>
       <c r="X12" s="8">
         <v>-504616419.17808223</v>
@@ -1775,14 +1774,14 @@
       <c r="AA12" s="8">
         <v>319153.42465753428</v>
       </c>
-      <c r="AB12" s="9" t="s">
-        <v>27</v>
+      <c r="AB12" s="9">
+        <v>0</v>
       </c>
       <c r="AC12" s="8">
         <v>1063619.1780821919</v>
       </c>
-      <c r="AD12" s="9" t="s">
-        <v>27</v>
+      <c r="AD12" s="9">
+        <v>0</v>
       </c>
       <c r="AE12" s="8">
         <v>-507704364.38356167</v>
@@ -1852,17 +1851,17 @@
       <c r="S13" s="8">
         <v>7836506.8493150687</v>
       </c>
-      <c r="T13" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U13" s="9" t="s">
-        <v>27</v>
+      <c r="T13" s="9">
+        <v>0</v>
+      </c>
+      <c r="U13" s="9">
+        <v>0</v>
       </c>
       <c r="V13" s="8">
         <v>450706054.79452056</v>
       </c>
-      <c r="W13" s="9" t="s">
-        <v>27</v>
+      <c r="W13" s="9">
+        <v>0</v>
       </c>
       <c r="X13" s="8">
         <v>-442869547.94520545</v>
@@ -1876,14 +1875,14 @@
       <c r="AA13" s="8">
         <v>991383.56164383562</v>
       </c>
-      <c r="AB13" s="9" t="s">
-        <v>27</v>
+      <c r="AB13" s="9">
+        <v>0</v>
       </c>
       <c r="AC13" s="8">
         <v>533547.94520547939</v>
       </c>
-      <c r="AD13" s="9" t="s">
-        <v>27</v>
+      <c r="AD13" s="9">
+        <v>0</v>
       </c>
       <c r="AE13" s="8">
         <v>-446131410.95890415</v>
@@ -1953,17 +1952,17 @@
       <c r="S14" s="9">
         <v>10375000</v>
       </c>
-      <c r="T14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U14" s="9" t="s">
-        <v>27</v>
+      <c r="T14" s="9">
+        <v>0</v>
+      </c>
+      <c r="U14" s="9">
+        <v>0</v>
       </c>
       <c r="V14" s="9">
         <v>392840000</v>
       </c>
-      <c r="W14" s="9" t="s">
-        <v>27</v>
+      <c r="W14" s="9">
+        <v>0</v>
       </c>
       <c r="X14" s="9">
         <v>-382465000</v>
@@ -1977,14 +1976,14 @@
       <c r="AA14" s="9">
         <v>1649000</v>
       </c>
-      <c r="AB14" s="9" t="s">
-        <v>27</v>
+      <c r="AB14" s="9">
+        <v>0</v>
       </c>
       <c r="AC14" s="9">
         <v>15000</v>
       </c>
-      <c r="AD14" s="9" t="s">
-        <v>27</v>
+      <c r="AD14" s="9">
+        <v>0</v>
       </c>
       <c r="AE14" s="9">
         <v>-385897000</v>
@@ -2054,17 +2053,17 @@
       <c r="S15" s="8">
         <v>46899657.534246564</v>
       </c>
-      <c r="T15" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U15" s="9" t="s">
-        <v>27</v>
+      <c r="T15" s="9">
+        <v>0</v>
+      </c>
+      <c r="U15" s="9">
+        <v>0</v>
       </c>
       <c r="V15" s="8">
         <v>412474808.21917808</v>
       </c>
-      <c r="W15" s="9" t="s">
-        <v>27</v>
+      <c r="W15" s="9">
+        <v>0</v>
       </c>
       <c r="X15" s="8">
         <v>-365575150.68493158</v>
@@ -2078,14 +2077,14 @@
       <c r="AA15" s="8">
         <v>864156.1643835617</v>
       </c>
-      <c r="AB15" s="9" t="s">
-        <v>27</v>
+      <c r="AB15" s="9">
+        <v>0</v>
       </c>
       <c r="AC15" s="8">
         <v>71594.520547945198</v>
       </c>
-      <c r="AD15" s="9" t="s">
-        <v>27</v>
+      <c r="AD15" s="9">
+        <v>0</v>
       </c>
       <c r="AE15" s="8">
         <v>-564896243.83561635</v>
@@ -2155,17 +2154,17 @@
       <c r="S16" s="8">
         <v>83825684.931506842</v>
       </c>
-      <c r="T16" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U16" s="9" t="s">
-        <v>27</v>
+      <c r="T16" s="9">
+        <v>0</v>
+      </c>
+      <c r="U16" s="9">
+        <v>0</v>
       </c>
       <c r="V16" s="8">
         <v>432325383.56164384</v>
       </c>
-      <c r="W16" s="9" t="s">
-        <v>27</v>
+      <c r="W16" s="9">
+        <v>0</v>
       </c>
       <c r="X16" s="8">
         <v>-348499698.63013703</v>
@@ -2179,14 +2178,14 @@
       <c r="AA16" s="8">
         <v>70687.671232876717</v>
       </c>
-      <c r="AB16" s="9" t="s">
-        <v>27</v>
+      <c r="AB16" s="9">
+        <v>0</v>
       </c>
       <c r="AC16" s="8">
         <v>128810.95890410959</v>
       </c>
-      <c r="AD16" s="9" t="s">
-        <v>27</v>
+      <c r="AD16" s="9">
+        <v>0</v>
       </c>
       <c r="AE16" s="8">
         <v>-745862512.32876706</v>
@@ -2256,17 +2255,17 @@
       <c r="S17" s="8">
         <v>120751712.32876711</v>
       </c>
-      <c r="T17" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U17" s="9" t="s">
-        <v>27</v>
+      <c r="T17" s="9">
+        <v>0</v>
+      </c>
+      <c r="U17" s="9">
+        <v>0</v>
       </c>
       <c r="V17" s="8">
         <v>452175958.9041096</v>
       </c>
-      <c r="W17" s="9" t="s">
-        <v>27</v>
+      <c r="W17" s="9">
+        <v>0</v>
       </c>
       <c r="X17" s="8">
         <v>-331424246.57534248</v>
@@ -2280,14 +2279,14 @@
       <c r="AA17" s="8">
         <v>-722780.82191780827</v>
       </c>
-      <c r="AB17" s="9" t="s">
-        <v>27</v>
+      <c r="AB17" s="9">
+        <v>0</v>
       </c>
       <c r="AC17" s="8">
         <v>186027.39726027398</v>
       </c>
-      <c r="AD17" s="9" t="s">
-        <v>27</v>
+      <c r="AD17" s="9">
+        <v>0</v>
       </c>
       <c r="AE17" s="8">
         <v>-926828780.82191777</v>
@@ -2357,17 +2356,17 @@
       <c r="S18" s="8">
         <v>156875000</v>
       </c>
-      <c r="T18" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="U18" s="8" t="s">
-        <v>27</v>
+      <c r="T18" s="9">
+        <v>0</v>
+      </c>
+      <c r="U18" s="9">
+        <v>0</v>
       </c>
       <c r="V18" s="8">
         <v>471595000</v>
       </c>
-      <c r="W18" s="8" t="s">
-        <v>27</v>
+      <c r="W18" s="9">
+        <v>0</v>
       </c>
       <c r="X18" s="8">
         <v>-314720000</v>
@@ -2381,14 +2380,14 @@
       <c r="AA18" s="8">
         <v>-1499000</v>
       </c>
-      <c r="AB18" s="8" t="s">
-        <v>27</v>
+      <c r="AB18" s="9">
+        <v>0</v>
       </c>
       <c r="AC18" s="8">
         <v>242000</v>
       </c>
-      <c r="AD18" s="8" t="s">
-        <v>27</v>
+      <c r="AD18" s="9">
+        <v>0</v>
       </c>
       <c r="AE18" s="8">
         <v>-1103861000</v>

</xml_diff>